<commit_message>
exploration on oil dataset from literature
</commit_message>
<xml_diff>
--- a/data/2024/species24.xlsx
+++ b/data/2024/species24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/data/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{1893269F-7BB5-437A-BD0F-7FBCB873B4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1F8A723-9C63-456E-AE26-6172BB430EA6}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{1893269F-7BB5-437A-BD0F-7FBCB873B4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B32A2AFF-6166-4336-B86D-A639AECA15FA}"/>
   <bookViews>
-    <workbookView xWindow="-22950" yWindow="0" windowWidth="17985" windowHeight="15540" xr2:uid="{CC4B9B15-E2AD-4C5C-96F0-50B6E9201024}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC4B9B15-E2AD-4C5C-96F0-50B6E9201024}"/>
   </bookViews>
   <sheets>
     <sheet name="species24" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>code</t>
   </si>
@@ -104,9 +104,6 @@
     <t>070823-09</t>
   </si>
   <si>
-    <t>040822-04</t>
-  </si>
-  <si>
     <t>210823-01</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>Jurinea humilis</t>
   </si>
   <si>
-    <t>Luzula caespitosa</t>
-  </si>
-  <si>
     <t>Minuartia verna</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>Brassicaceae</t>
   </si>
   <si>
-    <t>Juncaceae</t>
-  </si>
-  <si>
     <t>Saxifragaceae</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
   </si>
   <si>
     <t>Jurihumi</t>
-  </si>
-  <si>
-    <t>Luzucaes</t>
   </si>
   <si>
     <t>Minuvern</t>
@@ -234,7 +222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,13 +244,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Aptos Display"/>
       <family val="2"/>
@@ -271,13 +252,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -303,25 +277,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -663,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2739B9DC-C670-4FD4-A02C-DF45448E90F1}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,13 +651,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -698,18 +666,18 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -718,24 +686,24 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -748,14 +716,14 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -771,14 +739,14 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -794,37 +762,37 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -840,14 +808,14 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -863,92 +831,92 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>35</v>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
         <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -958,45 +926,22 @@
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ordering data cleaning scripts intro and methods more detailed
</commit_message>
<xml_diff>
--- a/data/2024/species24.xlsx
+++ b/data/2024/species24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/data/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{1893269F-7BB5-437A-BD0F-7FBCB873B4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B32A2AFF-6166-4336-B86D-A639AECA15FA}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{1893269F-7BB5-437A-BD0F-7FBCB873B4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48EE7C3A-7694-4FD6-A321-430F4DC2A08D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC4B9B15-E2AD-4C5C-96F0-50B6E9201024}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC4B9B15-E2AD-4C5C-96F0-50B6E9201024}"/>
   </bookViews>
   <sheets>
     <sheet name="species24" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Specialist</t>
-  </si>
-  <si>
     <t>Caryophyllaceae</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>family</t>
+  </si>
+  <si>
+    <t>Strict alpine</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,13 +651,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -666,44 +666,44 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -712,21 +712,21 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -735,21 +735,21 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -758,136 +758,136 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
       </c>
       <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -896,53 +896,53 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>